<commit_message>
Se completó la carga de datosp or medio de archivo plano
</commit_message>
<xml_diff>
--- a/src/AppBundle/Resources/public/template/importar.template.xlsx
+++ b/src/AppBundle/Resources/public/template/importar.template.xlsx
@@ -19,9 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
-  <si>
-    <t xml:space="preserve">no elimine esta fila. Campos con * son obligatorios. Los campos referencia de la base de datos deben estar tal y como aparecen en la base de datos. </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+  <si>
+    <t>no elimine estas filas. Campos con * son obligatorios. Los campos referencia de la base de datos deben estar tal y como aparecen en la base de datos.  No modifique los nombres de las columnas</t>
   </si>
   <si>
     <t>INFORMACIÓN GENERAL</t>
@@ -40,6 +40,66 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>* Tal y como aparece en listado de seccionales del sistema</t>
+  </si>
+  <si>
+    <t>* Tal y como aparece en el listado de tipos de solicitud del sistema</t>
+  </si>
+  <si>
+    <t>* Tal y como aparece en el listado de grados del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de unidades del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de antiguedad del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de cantida de población a beneficiar del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparecen en el listado de población a beneficiar del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de zonas ubicación del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de cantidad de beneficios institucionales del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de parentescos del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de estados civiles del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de ingresos del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de personas a cargo del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de situaciones de vivienda del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de dificultades del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de cantidad de beneficios AOS del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de conceptos de visita domiciliaria del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de afiliado a DIBIE del sistema</t>
+  </si>
+  <si>
+    <t>* Tal y como aparece en el listado de areas del sistema</t>
+  </si>
+  <si>
+    <t>* Tal y como aparece en el listado de programas del sistema</t>
   </si>
   <si>
     <t>FECHA_DE_SOLICITUD</t>
@@ -155,11 +215,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -196,8 +256,129 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -211,130 +392,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -349,61 +409,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -415,121 +571,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -574,8 +634,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -585,6 +645,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,26 +694,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -654,161 +720,155 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -847,17 +907,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="37" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1208,10 +1268,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -1229,18 +1289,25 @@
     <col min="11" max="11" width="9" style="17" customWidth="1"/>
     <col min="12" max="12" width="33.4266666666667" style="17" customWidth="1"/>
     <col min="13" max="13" width="23.7" style="16" customWidth="1"/>
-    <col min="14" max="14" width="29.6" style="16" customWidth="1"/>
-    <col min="15" max="15" width="20.8" style="16" customWidth="1"/>
+    <col min="14" max="14" width="33.8" style="16" customWidth="1"/>
+    <col min="15" max="15" width="24.3" style="16" customWidth="1"/>
     <col min="16" max="16" width="15.1" style="16" customWidth="1"/>
-    <col min="17" max="17" width="39.7" style="16" customWidth="1"/>
+    <col min="17" max="17" width="35.7333333333333" style="16" customWidth="1"/>
     <col min="18" max="18" width="26" style="16" customWidth="1"/>
-    <col min="19" max="20" width="11.4266666666667" style="16"/>
+    <col min="19" max="19" width="13.8" style="16" customWidth="1"/>
+    <col min="20" max="20" width="10.2" style="16" customWidth="1"/>
     <col min="21" max="21" width="18.1" style="16" customWidth="1"/>
-    <col min="22" max="22" width="17.9" style="16" customWidth="1"/>
-    <col min="23" max="16384" width="11.4266666666667" style="16"/>
+    <col min="22" max="22" width="20.7" style="16" customWidth="1"/>
+    <col min="23" max="23" width="11.4266666666667" style="16"/>
+    <col min="24" max="24" width="26.8" style="16" customWidth="1"/>
+    <col min="25" max="25" width="31.8" style="16" customWidth="1"/>
+    <col min="26" max="26" width="15.2" style="16" customWidth="1"/>
+    <col min="27" max="27" width="32.8" style="16" customWidth="1"/>
+    <col min="28" max="28" width="29" style="16" customWidth="1"/>
+    <col min="29" max="16384" width="11.4266666666667" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" ht="63.75" spans="1:31">
+    <row r="1" ht="76.5" spans="1:30">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1253,186 +1320,213 @@
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23" t="s">
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23" t="s">
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="26" t="s">
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" ht="102" spans="1:30">
       <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="E2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="F2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="G2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="H2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="I2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="23"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="23"/>
-      <c r="AC2" s="23"/>
-      <c r="AD2" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE2" s="26" t="s">
-        <v>6</v>
+      <c r="J2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="X2" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y2" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z2" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD2" s="20" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="3" ht="16.5" customHeight="1" spans="1:31">
-      <c r="A3" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="22" t="s">
-        <v>18</v>
+    <row r="3" ht="16.5" customHeight="1" spans="1:30">
+      <c r="A3" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="M3" s="24" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="N3" s="24" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="O3" s="24" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="P3" s="24" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="Q3" s="24" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="R3" s="24" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="S3" s="24" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="T3" s="24" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="U3" s="24" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="V3" s="24" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="W3" s="24" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="X3" s="24" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="Y3" s="24" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="Z3" s="24" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="AA3" s="24" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="AB3" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC3" s="24"/>
+        <v>54</v>
+      </c>
+      <c r="AC3" s="24" t="s">
+        <v>55</v>
+      </c>
       <c r="AD3" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE3" s="24" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1443,7 +1537,7 @@
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:AC1"/>
+    <mergeCell ref="R1:AB1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" scale="95" orientation="portrait"/>
@@ -1477,7 +1571,7 @@
     <row r="2" spans="1:4">
       <c r="A2" s="3"/>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1493,7 +1587,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C4" s="9">
         <v>2000</v>
@@ -1510,7 +1604,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C5" s="9">
         <v>80000</v>
@@ -1527,7 +1621,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C6" s="9">
         <v>26000</v>
@@ -1544,7 +1638,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C7" s="9">
         <v>5000</v>
@@ -1584,7 +1678,7 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="11" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="D11" s="12">
         <f>SUM(D4:D9)</f>

</xml_diff>

<commit_message>
Ajutes finales importar datos
</commit_message>
<xml_diff>
--- a/src/AppBundle/Resources/public/template/importar.template.xlsx
+++ b/src/AppBundle/Resources/public/template/importar.template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8310"/>
+    <workbookView windowWidth="19890" windowHeight="8310"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>no elimine estas filas. Campos con * son obligatorios. Los campos referencia de la base de datos deben estar tal y como aparecen en la base de datos.  No modifique los nombres de las columnas</t>
   </si>
@@ -57,46 +57,43 @@
     <t>Tal y como aparece en el listado de antiguedad del sistema</t>
   </si>
   <si>
-    <t>Tal y como aparece en el listado de cantida de población a beneficiar del sistema</t>
-  </si>
-  <si>
-    <t>Tal y como aparecen en el listado de población a beneficiar del sistema</t>
-  </si>
-  <si>
-    <t>Tal y como aparece en el listado de zonas ubicación del sistema</t>
+    <t>Tal y como aparece en el listado de parentescos del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparecen en el listado de estados civiles del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de ingresos del sistema</t>
   </si>
   <si>
     <t>Tal y como aparece en el listado de cantidad de beneficios institucionales del sistema</t>
   </si>
   <si>
-    <t>Tal y como aparece en el listado de parentescos del sistema</t>
+    <t>Tal y como aparece en el listado de personas a cargo del sistema</t>
   </si>
   <si>
     <t>Tal y como aparece en el listado de estados civiles del sistema</t>
   </si>
   <si>
-    <t>Tal y como aparece en el listado de ingresos del sistema</t>
-  </si>
-  <si>
-    <t>Tal y como aparece en el listado de personas a cargo del sistema</t>
-  </si>
-  <si>
-    <t>Tal y como aparece en el listado de situaciones de vivienda del sistema</t>
-  </si>
-  <si>
-    <t>Tal y como aparece en el listado de dificultades del sistema</t>
-  </si>
-  <si>
-    <t>Tal y como aparece en el listado de cantidad de beneficios AOS del sistema</t>
+    <t>Tal y como aparece en el listado decantidad de beneficios aos del sistema</t>
   </si>
   <si>
     <t>Tal y como aparece en el listado de conceptos de visita domiciliaria del sistema</t>
   </si>
   <si>
-    <t>Tal y como aparece en el listado de afiliado a DIBIE del sistema</t>
-  </si>
-  <si>
-    <t>* Tal y como aparece en el listado de areas del sistema</t>
+    <t>Tal y como aparece en el listado de afiliacion a DIBIE del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de cantidad de poblacion a beneficiar del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como aparece en el listado de viabilidad planeacion del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como a parece en el listado de zonas de ubicacion del sistema</t>
+  </si>
+  <si>
+    <t>Tal y como a parece en el listado de cantidad de beneficios institucionales del sistema</t>
   </si>
   <si>
     <t>* Tal y como aparece en el listado de programas del sistema</t>
@@ -126,6 +123,9 @@
     <t>TELEFONO</t>
   </si>
   <si>
+    <t>TELEFONO_ALTERNO</t>
+  </si>
+  <si>
     <t>CEDULA_FUNCIONARIO_POLICIAL</t>
   </si>
   <si>
@@ -141,6 +141,39 @@
     <t>ANTIGUEDAD_FUNCIONARIO</t>
   </si>
   <si>
+    <t>PARENTESCO_SOLICITANTE</t>
+  </si>
+  <si>
+    <t>ESTADO_CIVIL</t>
+  </si>
+  <si>
+    <t>INGRESOS</t>
+  </si>
+  <si>
+    <t>PERSONAS_A_CARGO</t>
+  </si>
+  <si>
+    <t>SITUACION_VIVIENDA</t>
+  </si>
+  <si>
+    <t>DIFICULTAD</t>
+  </si>
+  <si>
+    <t>CANTIDAD_BENEFICIOS_AOS</t>
+  </si>
+  <si>
+    <t>CONCEPTO_VISITA_DOMICILIARIA</t>
+  </si>
+  <si>
+    <t>AFILIADO_DIBIE</t>
+  </si>
+  <si>
+    <t>DOCUMENTO_BENEFICIARIO_FINAL</t>
+  </si>
+  <si>
+    <t>NOMBRE_BENEFICIARIO_FINAL</t>
+  </si>
+  <si>
     <t>CANTIDAD_POBLACION_BENEFICIAR</t>
   </si>
   <si>
@@ -153,40 +186,7 @@
     <t>CANTIDAD_BENEFICIOS_INSTITUCIONALES</t>
   </si>
   <si>
-    <t>PARENTESCO_SOLICITANTE</t>
-  </si>
-  <si>
-    <t>ESTADO_CIVIL</t>
-  </si>
-  <si>
-    <t>INGRESOS</t>
-  </si>
-  <si>
-    <t>PERSONAS_A_CARGO</t>
-  </si>
-  <si>
-    <t>SITUACION_VIVIENDA</t>
-  </si>
-  <si>
-    <t>DIFICULTAD</t>
-  </si>
-  <si>
-    <t>CANTIDAD_BENEFICIOS_AOS</t>
-  </si>
-  <si>
-    <t>CONCEPTO_VISITA_DOMICILIARIA</t>
-  </si>
-  <si>
-    <t>AFILIADO_DIBIE</t>
-  </si>
-  <si>
-    <t>DOCUMENTO_BENEFICIARIO_FINAL</t>
-  </si>
-  <si>
-    <t>NOMBRE_BENEFICIARIO_FINAL</t>
-  </si>
-  <si>
-    <t>AREA</t>
+    <t>DESCRIPCION_SOLICITUD</t>
   </si>
   <si>
     <t>PROGRAMAS</t>
@@ -214,14 +214,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,12 +251,37 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <name val="DejaVu Sans Mono"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial Narrow"/>
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -264,45 +290,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -317,59 +329,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -377,6 +336,59 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -385,16 +397,30 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -409,96 +435,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -506,90 +616,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -634,32 +660,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -694,17 +711,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -724,155 +741,164 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -896,6 +922,7 @@
     <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="37" applyFont="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -910,15 +937,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="37" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1268,276 +1302,317 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" outlineLevelRow="3"/>
   <cols>
     <col min="1" max="1" width="31.8" style="14" customWidth="1"/>
-    <col min="2" max="2" width="11.1" style="14" customWidth="1"/>
-    <col min="3" max="3" width="15.7" style="15" customWidth="1"/>
-    <col min="4" max="4" width="21" style="16" customWidth="1"/>
-    <col min="5" max="5" width="33.8" style="16" customWidth="1"/>
-    <col min="6" max="6" width="6.6" style="16" customWidth="1"/>
-    <col min="7" max="7" width="11.9" style="17" customWidth="1"/>
-    <col min="8" max="8" width="11.4" style="17" customWidth="1"/>
-    <col min="9" max="9" width="28.9533333333333" style="17" customWidth="1"/>
-    <col min="10" max="10" width="27.9933333333333" style="17" customWidth="1"/>
-    <col min="11" max="11" width="9" style="17" customWidth="1"/>
-    <col min="12" max="12" width="33.4266666666667" style="17" customWidth="1"/>
-    <col min="13" max="13" width="23.7" style="16" customWidth="1"/>
-    <col min="14" max="14" width="33.8" style="16" customWidth="1"/>
-    <col min="15" max="15" width="24.3" style="16" customWidth="1"/>
-    <col min="16" max="16" width="15.1" style="16" customWidth="1"/>
-    <col min="17" max="17" width="35.7333333333333" style="16" customWidth="1"/>
-    <col min="18" max="18" width="26" style="16" customWidth="1"/>
-    <col min="19" max="19" width="13.8" style="16" customWidth="1"/>
-    <col min="20" max="20" width="10.2" style="16" customWidth="1"/>
-    <col min="21" max="21" width="18.1" style="16" customWidth="1"/>
-    <col min="22" max="22" width="20.7" style="16" customWidth="1"/>
-    <col min="23" max="23" width="11.4266666666667" style="16"/>
-    <col min="24" max="24" width="26.8" style="16" customWidth="1"/>
-    <col min="25" max="25" width="31.8" style="16" customWidth="1"/>
-    <col min="26" max="26" width="15.2" style="16" customWidth="1"/>
-    <col min="27" max="27" width="32.8" style="16" customWidth="1"/>
-    <col min="28" max="28" width="29" style="16" customWidth="1"/>
-    <col min="29" max="16384" width="11.4266666666667" style="16"/>
+    <col min="2" max="2" width="11.1" style="15" customWidth="1"/>
+    <col min="3" max="3" width="15.7" style="16" customWidth="1"/>
+    <col min="4" max="4" width="21" style="17" customWidth="1"/>
+    <col min="5" max="5" width="33.8" style="17" customWidth="1"/>
+    <col min="6" max="6" width="6.6" style="17" customWidth="1"/>
+    <col min="7" max="8" width="11.9" style="18" customWidth="1"/>
+    <col min="9" max="9" width="18.7" style="18" customWidth="1"/>
+    <col min="10" max="10" width="28.9533333333333" style="18" customWidth="1"/>
+    <col min="11" max="11" width="27.9933333333333" style="18" customWidth="1"/>
+    <col min="12" max="12" width="9" style="18" customWidth="1"/>
+    <col min="13" max="13" width="33.4266666666667" style="18" customWidth="1"/>
+    <col min="14" max="14" width="23.7" style="17" customWidth="1"/>
+    <col min="15" max="15" width="33.8" style="17" customWidth="1"/>
+    <col min="16" max="16" width="24.3" style="17" customWidth="1"/>
+    <col min="17" max="17" width="15.1" style="17" customWidth="1"/>
+    <col min="18" max="18" width="35.7333333333333" style="17" customWidth="1"/>
+    <col min="19" max="19" width="26" style="17" customWidth="1"/>
+    <col min="20" max="20" width="13.8" style="17" customWidth="1"/>
+    <col min="21" max="21" width="22.9" style="17" customWidth="1"/>
+    <col min="22" max="22" width="27.8" style="17" customWidth="1"/>
+    <col min="23" max="23" width="20.7" style="17" customWidth="1"/>
+    <col min="24" max="24" width="27.8" style="17" customWidth="1"/>
+    <col min="25" max="25" width="26.8" style="17" customWidth="1"/>
+    <col min="26" max="26" width="31.8" style="17" customWidth="1"/>
+    <col min="27" max="27" width="21" style="17" customWidth="1"/>
+    <col min="28" max="28" width="32.8" style="17" customWidth="1"/>
+    <col min="29" max="29" width="29" style="17" customWidth="1"/>
+    <col min="30" max="30" width="24" style="17" customWidth="1"/>
+    <col min="31" max="31" width="12.5" style="17" customWidth="1"/>
+    <col min="32" max="32" width="11.7" style="17" customWidth="1"/>
+    <col min="33" max="16384" width="11.4266666666667" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" ht="76.5" spans="1:30">
-      <c r="A1" s="18" t="s">
+    <row r="1" ht="76.5" spans="1:31">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19" t="s">
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19" t="s">
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="20" t="s">
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="102" spans="1:30">
-      <c r="A2" s="18" t="s">
+    <row r="2" ht="102" spans="1:31">
+      <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="J2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="K2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="L2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="21"/>
+      <c r="N2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="O2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="20" t="s">
+      <c r="P2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="20" t="s">
+      <c r="Q2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="20" t="s">
+      <c r="R2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="20" t="s">
+      <c r="S2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="20" t="s">
+      <c r="T2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="20" t="s">
+      <c r="U2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="20" t="s">
+      <c r="V2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="20" t="s">
+      <c r="W2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="20" t="s">
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="20" t="s">
+      <c r="AA2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" s="20" t="s">
+      <c r="AB2" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" s="20" t="s">
+      <c r="AC2" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="26" t="s">
+      <c r="AD2" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE2" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="AD2" s="20" t="s">
+    </row>
+    <row r="3" ht="16.5" customHeight="1" spans="1:32">
+      <c r="A3" s="22" t="s">
         <v>26</v>
       </c>
+      <c r="B3" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="S3" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="U3" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="V3" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="W3" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="X3" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y3" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z3" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA3" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB3" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC3" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD3" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE3" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF3" s="28"/>
     </row>
-    <row r="3" ht="16.5" customHeight="1" spans="1:30">
-      <c r="A3" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="O3" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="P3" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q3" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="R3" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="S3" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="T3" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="U3" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="V3" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="W3" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="X3" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y3" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z3" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA3" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB3" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC3" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD3" s="24" t="s">
-        <v>56</v>
-      </c>
+    <row r="4" ht="43" customHeight="1" spans="1:31">
+      <c r="A4" s="23"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="24"/>
+      <c r="AD4" s="24"/>
+      <c r="AE4" s="24"/>
     </row>
   </sheetData>
-  <sortState ref="A4:J1877">
+  <sortState ref="A4:K1877">
     <sortCondition ref="D4:D1877"/>
   </sortState>
   <mergeCells count="4">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="I1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:AB1"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="S1:AC1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" scale="95" orientation="portrait"/>

</xml_diff>